<commit_message>
Completed create newencounter test case
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\CoCareTestAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334C4229-2AB0-46B6-9EC0-F7F5A2EDD5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F12C29-D0A2-4C48-82F4-AF51C1187139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D48CD984-6211-407B-BF54-5877E2F3739C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>pScriptName</t>
   </si>
@@ -78,9 +78,6 @@
     <t>cocareproject2024+ncmtest1@gmail.com</t>
   </si>
   <si>
-    <t>08/08/2024</t>
-  </si>
-  <si>
     <t>abc</t>
   </si>
   <si>
@@ -118,6 +115,15 @@
   </si>
   <si>
     <t xml:space="preserve">Yes. Received dose in hand </t>
+  </si>
+  <si>
+    <t>pOverdoseDate</t>
+  </si>
+  <si>
+    <t>08-08-2024</t>
+  </si>
+  <si>
+    <t>pContingency</t>
   </si>
 </sst>
 </file>
@@ -6934,7 +6940,7 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="56" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6953,9 +6959,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5854">
     <cellStyle name="20% - Accent1" xfId="14" builtinId="30" customBuiltin="1"/>
@@ -13123,10 +13126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69904A16-BBAB-48A8-A4C3-C9CA1CCECF6C}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13135,9 +13138,10 @@
     <col min="2" max="2" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" style="8"/>
+    <col min="12" max="12" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13163,22 +13167,28 @@
         <v>11</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>21</v>
+      <c r="J1" s="5" t="s">
+        <v>24</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="K1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="10" t="s">
-        <v>26</v>
+      <c r="L1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -13189,7 +13199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -13200,7 +13210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -13211,52 +13221,58 @@
         <v>3</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
-      <c r="L4" t="s">
-        <v>22</v>
+      <c r="L4" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:15">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:15">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:15">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:15">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:15">
       <c r="A9" s="2"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:15">
       <c r="A11" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated all new authentication scripts
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\CoCareTestAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F12C29-D0A2-4C48-82F4-AF51C1187139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAB84F6-8B9D-4D24-8CCB-9D22667AA472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D48CD984-6211-407B-BF54-5877E2F3739C}"/>
+    <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="8170" xr2:uid="{D48CD984-6211-407B-BF54-5877E2F3739C}"/>
   </bookViews>
   <sheets>
     <sheet name="InputData" sheetId="1" r:id="rId1"/>
@@ -34,21 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>pScriptName</t>
-  </si>
-  <si>
-    <t>LoginWithValidCredentials</t>
-  </si>
-  <si>
-    <t>cocareproject2024@gmail.com</t>
-  </si>
-  <si>
-    <t>Eclipse$2024</t>
-  </si>
-  <si>
-    <t>ValidateAuthenticationInvalidCredential</t>
   </si>
   <si>
     <t>puseremail</t>
@@ -75,12 +63,6 @@
     <t>CreateNewEncounter</t>
   </si>
   <si>
-    <t>cocareproject2024+ncmtest1@gmail.com</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
     <t>Stevenson Family Health Center-Bronx-NY</t>
   </si>
   <si>
@@ -91,9 +73,6 @@
   </si>
   <si>
     <t>pEncounterType</t>
-  </si>
-  <si>
-    <t>1234</t>
   </si>
   <si>
     <t>pUrineDrugTest</t>
@@ -120,10 +99,61 @@
     <t>pOverdoseDate</t>
   </si>
   <si>
-    <t>08-08-2024</t>
+    <t>pContingency</t>
   </si>
   <si>
-    <t>pContingency</t>
+    <t>08-25-2024</t>
+  </si>
+  <si>
+    <t>John Physician</t>
+  </si>
+  <si>
+    <t>CreateEncounterforInprogressParticipant</t>
+  </si>
+  <si>
+    <t>pregistryid</t>
+  </si>
+  <si>
+    <t>cocareproject2024+ncmtest1@gmail.com</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <t>AutoTest234</t>
+  </si>
+  <si>
+    <t>cocareproject2024@gmail.com</t>
+  </si>
+  <si>
+    <t>AccountLockedDuetoInactivity</t>
+  </si>
+  <si>
+    <t>padminuseremail</t>
+  </si>
+  <si>
+    <t>padminpassword</t>
+  </si>
+  <si>
+    <t>Location$2024</t>
+  </si>
+  <si>
+    <t>ValidatePasswordComplexity</t>
+  </si>
+  <si>
+    <t>AccountLockedDuetoExpiredPassword</t>
+  </si>
+  <si>
+    <t>AccountLockedDuetoFailedattempts</t>
+  </si>
+  <si>
+    <t>ValidateAdminPagePasswordComplexity</t>
+  </si>
+  <si>
+    <t>ValidatePasswordExpiryWarning</t>
+  </si>
+  <si>
+    <t>ValidatePasswordResetAttempt</t>
   </si>
 </sst>
 </file>
@@ -6940,7 +6970,7 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="56" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6959,6 +6989,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="5854">
     <cellStyle name="20% - Accent1" xfId="14" builtinId="30" customBuiltin="1"/>
@@ -13126,161 +13157,254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69904A16-BBAB-48A8-A4C3-C9CA1CCECF6C}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="8"/>
-    <col min="12" max="12" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" style="8" customWidth="1"/>
+    <col min="15" max="15" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>8</v>
+      <c r="L1" s="5" t="s">
+        <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
+      <c r="M1" s="5" t="s">
+        <v>17</v>
       </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="R1" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="2"/>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="2"/>
+    <row r="3" spans="1:18">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="2"/>
+    <row r="4" spans="1:18">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="2"/>
+    <row r="5" spans="1:18">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="2"/>
+    <row r="6" spans="1:18">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="2"/>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="56" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B41A1091-0758-4B4B-AFF1-E85BDC0CA3F4}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{148D4CB3-F312-4F2A-A310-CDFA46773C81}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{2D00B414-90B3-4A3F-BAC8-0B670F6A0F6F}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{28C5058F-46C8-40D0-8FCA-E77FC14D2E47}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{7563E499-8BB6-4403-92D1-D1A449DE0C06}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{271F00F0-445D-48E4-B482-1B39AA562B31}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{A6CA7C3B-53B1-4976-9FA8-4CF1096B33C2}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{6CDA32B1-349F-4AED-B7D4-E04EDE068124}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>